<commit_message>
Added error handling for non-Facebook pages in visitFacebookAbout
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -962,10 +962,10 @@
         <v>Eunice J.</v>
       </c>
       <c r="D33" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E33" t="str">
-        <v>Error</v>
+        <v>(925) 462-7212</v>
       </c>
     </row>
     <row r="34">
@@ -979,10 +979,10 @@
         <v>Tom Ha</v>
       </c>
       <c r="D34" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E34" t="str">
-        <v>Error</v>
+        <v>925-433-7809</v>
       </c>
     </row>
     <row r="35">
@@ -1030,10 +1030,10 @@
         <v>Dr. Sonam Agarwal</v>
       </c>
       <c r="D37" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E37" t="str">
-        <v>Error</v>
+        <v>925-461-3100</v>
       </c>
     </row>
     <row r="38">
@@ -1064,10 +1064,10 @@
         <v>Dr. Francine Kitagawa</v>
       </c>
       <c r="D39" t="str">
-        <v>Error</v>
+        <v>dentist@pleasanton-dental.com</v>
       </c>
       <c r="E39" t="str">
-        <v>Error</v>
+        <v>2004-2025</v>
       </c>
     </row>
     <row r="40">
@@ -3254,7 +3254,7 @@
         <v>www.igasakidental.com</v>
       </c>
       <c r="C168" t="str" xml:space="preserve">
-        <v xml:space="preserve">Dr. Alan Igasaki_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Dr. Alan Igasaki_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Dr. Howard Igasaki</v>
       </c>
       <c r="D168" t="str">
@@ -3544,7 +3544,7 @@
         <v>nohonuevodental.com</v>
       </c>
       <c r="C185" t="str" xml:space="preserve">
-        <v xml:space="preserve">Mary Yazdan, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Mary Yazdan, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Dr. Hameed Nejat DMD</v>
       </c>
       <c r="D185" t="str">
@@ -3664,7 +3664,7 @@
         <v>www.ccdentalinc.com</v>
       </c>
       <c r="C192" t="str" xml:space="preserve">
-        <v xml:space="preserve">Robert Tingillian, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Robert Tingillian, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Tom Shanakian, DDS</v>
       </c>
       <c r="D192" t="str">

</xml_diff>

<commit_message>
validate all links before returning null when no emails found
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -1030,7 +1030,7 @@
         <v>Dr. Sonam Agarwal</v>
       </c>
       <c r="D37" t="str">
-        <v>No email found</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E37" t="str">
         <v>925-461-3100</v>
@@ -1183,10 +1183,10 @@
         <v>Kerry Andre, DDS and Kristie Judson, DDS</v>
       </c>
       <c r="D46" t="str">
-        <v>Error</v>
+        <v>info@pleasantonsmiles.com</v>
       </c>
       <c r="E46" t="str">
-        <v>Error</v>
+        <v>(925) 462-1990</v>
       </c>
     </row>
     <row r="47">
@@ -1234,10 +1234,10 @@
         <v>Tom Ha</v>
       </c>
       <c r="D49" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E49" t="str">
-        <v>Error</v>
+        <v>925-433-7809</v>
       </c>
     </row>
     <row r="50">
@@ -1302,10 +1302,10 @@
         <v>Dr Leena Tolani and Amitesh Patel</v>
       </c>
       <c r="D53" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E53" t="str">
-        <v>Error</v>
+        <v>9256009888</v>
       </c>
     </row>
     <row r="54">
@@ -1336,10 +1336,10 @@
         <v>Dr. Sowjanya Srikantam, DDS</v>
       </c>
       <c r="D55" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E55" t="str">
-        <v>Error</v>
+        <v>(925) 249-1130</v>
       </c>
     </row>
     <row r="56">
@@ -1370,10 +1370,10 @@
         <v>Reginal Hom, DDS</v>
       </c>
       <c r="D57" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E57" t="str">
-        <v>Error</v>
+        <v>214872808</v>
       </c>
     </row>
     <row r="58">
@@ -1387,10 +1387,10 @@
         <v>Dr Leena Tolani and Amitesh Patel</v>
       </c>
       <c r="D58" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E58" t="str">
-        <v>Error</v>
+        <v>9256009888</v>
       </c>
     </row>
     <row r="59">
@@ -1404,10 +1404,10 @@
         <v>Dr. Chaitra Bhat</v>
       </c>
       <c r="D59" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E59" t="str">
-        <v>Error</v>
+        <v>(925) 485-1172</v>
       </c>
     </row>
     <row r="60">
@@ -1438,10 +1438,10 @@
         <v>Jeffrey R. Clayton, DDS and Ron G. Takahashi, DDS, MD</v>
       </c>
       <c r="D61" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E61" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
     </row>
     <row r="62">
@@ -1455,10 +1455,10 @@
         <v>Dr. Veena Madhure</v>
       </c>
       <c r="D62" t="str">
-        <v>Error</v>
+        <v>contact@pearlsandteeth.com</v>
       </c>
       <c r="E62" t="str">
-        <v>Error</v>
+        <v>925-523-3864</v>
       </c>
     </row>
     <row r="63">
@@ -1472,10 +1472,10 @@
         <v>Dr. Tran</v>
       </c>
       <c r="D63" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E63" t="str">
-        <v>Error</v>
+        <v>(925) 846-6308</v>
       </c>
     </row>
     <row r="64">
@@ -1489,10 +1489,10 @@
         <v>Dr. Maggie Chao &amp; Dr. Olivia Nguyen</v>
       </c>
       <c r="D64" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E64" t="str">
-        <v>Error</v>
+        <v>925-425-7545</v>
       </c>
     </row>
     <row r="65">
@@ -1506,10 +1506,10 @@
         <v>Arnold B. Jacobs</v>
       </c>
       <c r="D65" t="str">
-        <v>Error</v>
+        <v>arnoldjacobsstaff@att.net</v>
       </c>
       <c r="E65" t="str">
-        <v>Error</v>
+        <v>(925)846-3968</v>
       </c>
     </row>
     <row r="66">
@@ -1523,10 +1523,10 @@
         <v>Dr. Kamlesh Jinjuwadia</v>
       </c>
       <c r="D66" t="str">
-        <v>Error</v>
+        <v>info@eastbaydental.com</v>
       </c>
       <c r="E66" t="str">
-        <v>Error</v>
+        <v>(510) 818-9000</v>
       </c>
     </row>
     <row r="67">
@@ -1693,10 +1693,10 @@
         <v>Dr. Norman Wong</v>
       </c>
       <c r="D76" t="str">
-        <v>Error</v>
+        <v>normanrwong@ymail.com</v>
       </c>
       <c r="E76" t="str">
-        <v>Error</v>
+        <v>(925) 846-5506</v>
       </c>
     </row>
     <row r="77">
@@ -1710,10 +1710,10 @@
         <v>Dr. Ihab M. Hanna</v>
       </c>
       <c r="D77" t="str">
-        <v>Error</v>
+        <v>info@redwoodcitydental.com</v>
       </c>
       <c r="E77" t="str">
-        <v>Error</v>
+        <v>(925) 551-6464</v>
       </c>
     </row>
     <row r="78">
@@ -1744,10 +1744,10 @@
         <v>Kerry Andre, DDS and Kristie Judson, DDS</v>
       </c>
       <c r="D79" t="str">
-        <v>Error</v>
+        <v>kjudson321@gmail.com</v>
       </c>
       <c r="E79" t="str">
-        <v>Error</v>
+        <v>925-462-1990</v>
       </c>
     </row>
     <row r="80">
@@ -1761,10 +1761,10 @@
         <v>Dr. Prajesh Desai</v>
       </c>
       <c r="D80" t="str">
-        <v>Error</v>
+        <v>dublinranchdental@yahoo.com</v>
       </c>
       <c r="E80" t="str">
-        <v>Error</v>
+        <v>(925) 999-9088</v>
       </c>
     </row>
     <row r="81">
@@ -1778,10 +1778,10 @@
         <v>Dr Leena Tolani and Amitesh Patel</v>
       </c>
       <c r="D81" t="str">
-        <v>Error</v>
+        <v>pleasantondds@gmail.com</v>
       </c>
       <c r="E81" t="str">
-        <v>Error</v>
+        <v>9256009888</v>
       </c>
     </row>
     <row r="82">
@@ -1795,10 +1795,10 @@
         <v>Joe Bauer</v>
       </c>
       <c r="D82" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E82" t="str">
-        <v>Error</v>
+        <v>(415) 380-3600</v>
       </c>
     </row>
     <row r="83">
@@ -1812,10 +1812,10 @@
         <v>Sunni G. Yoon</v>
       </c>
       <c r="D83" t="str">
-        <v>Error</v>
+        <v>syoondds@gmail.com</v>
       </c>
       <c r="E83" t="str">
-        <v>Error</v>
+        <v>(707) 422-7003</v>
       </c>
     </row>
     <row r="84">
@@ -1846,10 +1846,10 @@
         <v>Dr. Joyce A. Pangilinan</v>
       </c>
       <c r="D85" t="str">
-        <v>Error</v>
+        <v>fairfielddentists@smilegeneration.com</v>
       </c>
       <c r="E85" t="str">
-        <v>Error</v>
+        <v>707-399-9082</v>
       </c>
     </row>
     <row r="86">
@@ -1863,10 +1863,10 @@
         <v>Frank J. Chen, DDS, Judy Su, DDS</v>
       </c>
       <c r="D86" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E86" t="str">
-        <v>Error</v>
+        <v>(707) 716-1715</v>
       </c>
     </row>
     <row r="87">
@@ -1965,10 +1965,10 @@
         <v>Dr. Steve Galvan</v>
       </c>
       <c r="D92" t="str">
-        <v>Error</v>
+        <v>galvandentalcorporation@gmail.com</v>
       </c>
       <c r="E92" t="str">
-        <v>Error</v>
+        <v>(925)676-6363</v>
       </c>
     </row>
     <row r="93">
@@ -1982,10 +1982,10 @@
         <v>Dr. Victor Santos</v>
       </c>
       <c r="D93" t="str">
-        <v>Error</v>
+        <v>victodonto@msn.com</v>
       </c>
       <c r="E93" t="str">
-        <v>Error</v>
+        <v>99931-7003</v>
       </c>
     </row>
     <row r="94">
@@ -1999,10 +1999,10 @@
         <v>Frank J. Chen, DDS, Judy Su, DDS</v>
       </c>
       <c r="D94" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E94" t="str">
-        <v>Error</v>
+        <v>(409) 883-5300</v>
       </c>
     </row>
     <row r="95">
@@ -2033,10 +2033,10 @@
         <v>Navid Mehranpour</v>
       </c>
       <c r="D96" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E96" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
     </row>
     <row r="97">
@@ -2288,10 +2288,10 @@
         <v>Dr. Mohini Patel</v>
       </c>
       <c r="D111" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E111" t="str">
-        <v>Error</v>
+        <v>916-246-1502</v>
       </c>
     </row>
     <row r="112">
@@ -2339,10 +2339,10 @@
         <v>Dr. Rupinderjit Kaur DDS</v>
       </c>
       <c r="D114" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E114" t="str">
-        <v>Error</v>
+        <v>(916) 723-3368</v>
       </c>
     </row>
     <row r="115">
@@ -2458,10 +2458,10 @@
         <v>Dr. Megan Moshar</v>
       </c>
       <c r="D121" t="str">
-        <v>Error</v>
+        <v>dentistsofoldtorrance@smilegeneration.com</v>
       </c>
       <c r="E121" t="str">
-        <v>Error</v>
+        <v>(424) 320-6584</v>
       </c>
     </row>
     <row r="122">
@@ -2492,10 +2492,10 @@
         <v>Dr. Sahar and Dr. Reza Mehr</v>
       </c>
       <c r="D123" t="str">
-        <v>Error</v>
+        <v>mehr@sparklefamilydentist.com</v>
       </c>
       <c r="E123" t="str">
-        <v>Error</v>
+        <v>424-378-1168</v>
       </c>
     </row>
     <row r="124">
@@ -2611,10 +2611,10 @@
         <v>Dr. Rosario Holland</v>
       </c>
       <c r="D130" t="str">
-        <v>Error</v>
+        <v>clientservice@yourhealthcontact.com</v>
       </c>
       <c r="E130" t="str">
-        <v>Error</v>
+        <v>3633090</v>
       </c>
     </row>
     <row r="131">
@@ -2917,10 +2917,10 @@
         <v>Dr. Chip Houske</v>
       </c>
       <c r="D148" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E148" t="str">
-        <v>Error</v>
+        <v>(310) 782-2008</v>
       </c>
     </row>
     <row r="149">
@@ -2934,10 +2934,10 @@
         <v>Dr. Leah Chin</v>
       </c>
       <c r="D149" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E149" t="str">
-        <v>Error</v>
+        <v>(310) 328-9700</v>
       </c>
     </row>
     <row r="150">
@@ -2951,10 +2951,10 @@
         <v>Dr. Byron Kim</v>
       </c>
       <c r="D150" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E150" t="str">
-        <v>Error</v>
+        <v>310-534-3002</v>
       </c>
     </row>
     <row r="151">
@@ -3019,10 +3019,10 @@
         <v>Dr. Samuel Gabriel</v>
       </c>
       <c r="D154" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E154" t="str">
-        <v>Error</v>
+        <v>(310) 483-7779</v>
       </c>
     </row>
     <row r="155">
@@ -3053,10 +3053,10 @@
         <v>Fredrick P. Fruhling II</v>
       </c>
       <c r="D156" t="str">
-        <v>Error</v>
+        <v>support@dentalinsider.com</v>
       </c>
       <c r="E156" t="str">
-        <v>Error</v>
+        <v>(310) 320-3264</v>
       </c>
     </row>
     <row r="157">
@@ -3070,10 +3070,10 @@
         <v>Daryn T. Nishikawa, DDS</v>
       </c>
       <c r="D157" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E157" t="str">
-        <v>Error</v>
+        <v>(310) 543-1655</v>
       </c>
     </row>
     <row r="158">
@@ -3154,12 +3154,6 @@
       <c r="C162" t="str">
         <v>Dr. A. Alejandra Rodriguez, Dr. Maria Elena Rodriguez, Dr. Michelle Ikoma</v>
       </c>
-      <c r="D162" t="str">
-        <v>Error</v>
-      </c>
-      <c r="E162" t="str">
-        <v>Error</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
@@ -3172,10 +3166,10 @@
         <v>Dr. Louis Yang</v>
       </c>
       <c r="D163" t="str">
-        <v>Error</v>
+        <v>louis_yang2@yahoo.com</v>
       </c>
       <c r="E163" t="str">
-        <v>Error</v>
+        <v>94587-2743</v>
       </c>
     </row>
     <row r="164">
@@ -3254,14 +3248,14 @@
         <v>www.igasakidental.com</v>
       </c>
       <c r="C168" t="str" xml:space="preserve">
-        <v xml:space="preserve">Dr. Alan Igasaki_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Dr. Alan Igasaki_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Dr. Howard Igasaki</v>
       </c>
       <c r="D168" t="str">
-        <v>Error</v>
+        <v>smile@igasakidental.com</v>
       </c>
       <c r="E168" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
     </row>
     <row r="169">
@@ -3275,10 +3269,10 @@
         <v>Dr. Jason Yamada</v>
       </c>
       <c r="D169" t="str">
-        <v>Error</v>
+        <v>IPIofTorrance@gmail.com</v>
       </c>
       <c r="E169" t="str">
-        <v>Error</v>
+        <v>(310)320-5661</v>
       </c>
     </row>
     <row r="170">
@@ -3343,10 +3337,10 @@
         <v>Hazem M. Yousef</v>
       </c>
       <c r="D173" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E173" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
     </row>
     <row r="174">
@@ -3360,10 +3354,10 @@
         <v>Dr. Abraham</v>
       </c>
       <c r="D174" t="str">
-        <v>Error</v>
+        <v>WCDCustomerService@westcoastdental.com</v>
       </c>
       <c r="E174" t="str">
-        <v>Error</v>
+        <v>(888) 329-8111</v>
       </c>
     </row>
     <row r="175">
@@ -3394,10 +3388,10 @@
         <v>Dr. Hammad Shere</v>
       </c>
       <c r="D176" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E176" t="str">
-        <v>Error</v>
+        <v>(669) 209-9319</v>
       </c>
     </row>
     <row r="177">
@@ -3410,12 +3404,6 @@
       <c r="C177" t="str">
         <v>Dr. Myra P. Ermita</v>
       </c>
-      <c r="D177" t="str">
-        <v>Error</v>
-      </c>
-      <c r="E177" t="str">
-        <v>Error</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
@@ -3427,12 +3415,6 @@
       <c r="C178" t="str">
         <v>Gerald S. Watanabe, DDS</v>
       </c>
-      <c r="D178" t="str">
-        <v>Error</v>
-      </c>
-      <c r="E178" t="str">
-        <v>Error</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
@@ -3530,10 +3512,10 @@
         <v>Dr. Penn Soh</v>
       </c>
       <c r="D184" t="str">
-        <v>Error</v>
+        <v>info@nohosmilecenter.com</v>
       </c>
       <c r="E184" t="str">
-        <v>Error</v>
+        <v>(818) 505-0106</v>
       </c>
     </row>
     <row r="185" xml:space="preserve">
@@ -3544,7 +3526,7 @@
         <v>nohonuevodental.com</v>
       </c>
       <c r="C185" t="str" xml:space="preserve">
-        <v xml:space="preserve">Mary Yazdan, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Mary Yazdan, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Dr. Hameed Nejat DMD</v>
       </c>
       <c r="D185" t="str">
@@ -3664,14 +3646,14 @@
         <v>www.ccdentalinc.com</v>
       </c>
       <c r="C192" t="str" xml:space="preserve">
-        <v xml:space="preserve">Robert Tingillian, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Robert Tingillian, DDS_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 Tom Shanakian, DDS</v>
       </c>
       <c r="D192" t="str">
-        <v>Error</v>
+        <v>info@bookdok.com</v>
       </c>
       <c r="E192" t="str">
-        <v>Error</v>
+        <v>818-788-2023</v>
       </c>
     </row>
     <row r="193">
@@ -3719,10 +3701,10 @@
         <v>Dr. Andrew Park</v>
       </c>
       <c r="D195" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E195" t="str">
-        <v>Error</v>
+        <v>(559) 325-0700</v>
       </c>
     </row>
     <row r="196">
@@ -3736,10 +3718,10 @@
         <v>Dennis E. Shamlian</v>
       </c>
       <c r="D196" t="str">
-        <v>Error</v>
+        <v>dennisdentalcare@gmail.com</v>
       </c>
       <c r="E196" t="str">
-        <v>Error</v>
+        <v>(559) 570-6981</v>
       </c>
     </row>
     <row r="197">
@@ -3872,10 +3854,10 @@
         <v>Dr. Mojgan Ramezani, DDS</v>
       </c>
       <c r="D204" t="str">
-        <v>Error</v>
+        <v>plazadentalla@gmail.com</v>
       </c>
       <c r="E204" t="str">
-        <v>Error</v>
+        <v>(818) 426-6654</v>
       </c>
     </row>
     <row r="205">
@@ -3923,10 +3905,10 @@
         <v>Dr. Robert X.P. Cai</v>
       </c>
       <c r="D207" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E207" t="str">
-        <v>Error</v>
+        <v>213-680-2808</v>
       </c>
     </row>
     <row r="208">
@@ -3991,10 +3973,10 @@
         <v>Matthew A. Caligiuri, DDS</v>
       </c>
       <c r="D211" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E211" t="str">
-        <v>Error</v>
+        <v>(213) 534-6856</v>
       </c>
     </row>
     <row r="212">
@@ -4076,10 +4058,10 @@
         <v>Dr. Adam J. Geach D.M.D., M.D.SC.</v>
       </c>
       <c r="D216" t="str">
-        <v>Error</v>
+        <v>ajg@u.arizona.edu</v>
       </c>
       <c r="E216" t="str">
-        <v>Error</v>
+        <v>91302-3014</v>
       </c>
     </row>
     <row r="217">
@@ -4144,10 +4126,10 @@
         <v>Dr. Joon Y. Lee, Dr. Sung W. Lee, Dr. Sue Y. Lee</v>
       </c>
       <c r="D220" t="str">
-        <v>Error</v>
+        <v>NO FB PAGE</v>
       </c>
       <c r="E220" t="str">
-        <v>Error</v>
+        <v>0506627</v>
       </c>
     </row>
     <row r="221">
@@ -4178,10 +4160,10 @@
         <v>Angeles Constancia</v>
       </c>
       <c r="D222" t="str">
-        <v>Error</v>
+        <v>No email found</v>
       </c>
       <c r="E222" t="str">
-        <v>Error</v>
+        <v>No phone found</v>
       </c>
     </row>
     <row r="223">
@@ -4263,10 +4245,10 @@
         <v>Dr. Kambiz Mahdavi</v>
       </c>
       <c r="D227" t="str">
-        <v>Error</v>
+        <v>drmahdavi@skylinedental.com</v>
       </c>
       <c r="E227" t="str">
-        <v>Error</v>
+        <v>(805) 212-5091</v>
       </c>
     </row>
     <row r="228">

</xml_diff>